<commit_message>
[Silverfox] 부엉이, 고양이 01, 02 전투 A.I 검증
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/NPCTubeCooler.xlsx
+++ b/DesignDocs/VariableData/NPCTubeCooler.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84793A3D-0949-48FB-8FDC-E4534BFC8BC4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="8112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -312,7 +313,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -706,21 +707,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" customWidth="1"/>
+    <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +747,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7101</v>
       </c>
@@ -772,7 +773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7102</v>
       </c>
@@ -798,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7103</v>
       </c>
@@ -824,7 +825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7104</v>
       </c>
@@ -850,7 +851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7105</v>
       </c>
@@ -876,7 +877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7106</v>
       </c>
@@ -902,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7107</v>
       </c>
@@ -928,7 +929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7108</v>
       </c>
@@ -945,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <v>10</v>
@@ -954,7 +955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7109</v>
       </c>
@@ -980,7 +981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7110</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>7111</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>7112</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>7113</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>7114</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>7115</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>7116</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>7117</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>7118</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>7119</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>7120</v>
       </c>
@@ -1266,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>7121</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>7122</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>7123</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>7124</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>7125</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>7126</v>
       </c>
@@ -1422,7 +1423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>7127</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>7128</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>7129</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>7130</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>7131</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>7132</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>7133</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>7134</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>7135</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>7136</v>
       </c>
@@ -1683,7 +1684,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Silverfox] Ailly / DonCena / PitBull A.I 기본 구성
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/NPCTubeCooler.xlsx
+++ b/DesignDocs/VariableData/NPCTubeCooler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DD6185-E19E-4C2D-B1FD-134F1A16B3B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45E3277-4CD0-404B-89E0-35F6EA52A1C9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -720,7 +720,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -877,7 +877,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
         <v>10</v>
@@ -903,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2">
         <v>10</v>
@@ -990,93 +990,93 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>7110</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>7111</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>7112</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>7110</v>
+        <v>7113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -1085,7 +1085,7 @@
         <v>7</v>
       </c>
       <c r="F14">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>10</v>
@@ -1096,13 +1096,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>7111</v>
+        <v>7114</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -1122,13 +1122,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>7112</v>
+        <v>7115</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1148,13 +1148,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>7113</v>
+        <v>7116</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -1174,13 +1174,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>7114</v>
+        <v>7117</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -1189,7 +1189,7 @@
         <v>7</v>
       </c>
       <c r="F18">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>10</v>
@@ -1200,13 +1200,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>7115</v>
+        <v>7118</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -1215,7 +1215,7 @@
         <v>7</v>
       </c>
       <c r="F19">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>10</v>
@@ -1226,13 +1226,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>7116</v>
+        <v>7119</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>7117</v>
+        <v>7120</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>6</v>
@@ -1278,13 +1278,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>7118</v>
+        <v>7121</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
@@ -1304,13 +1304,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>7119</v>
+        <v>7122</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>6</v>
@@ -1330,13 +1330,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>7120</v>
+        <v>7123</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>6</v>
@@ -1356,13 +1356,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>7121</v>
+        <v>7124</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
@@ -1382,13 +1382,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>7122</v>
+        <v>7125</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
@@ -1408,13 +1408,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>7123</v>
+        <v>7126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>7124</v>
+        <v>7127</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
@@ -1460,13 +1460,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>7125</v>
+        <v>7128</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>6</v>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>7126</v>
+        <v>7129</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>6</v>
@@ -1512,13 +1512,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>7127</v>
+        <v>7130</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -1538,13 +1538,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>7128</v>
+        <v>7131</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>6</v>
@@ -1564,13 +1564,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>7129</v>
+        <v>7132</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>6</v>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>7130</v>
+        <v>7133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>6</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>7131</v>
+        <v>7134</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>6</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>7132</v>
+        <v>7135</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>6</v>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>7133</v>
+        <v>7136</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>6</v>
@@ -1692,82 +1692,82 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>7134</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38">
-        <v>0.1</v>
-      </c>
-      <c r="G38">
-        <v>10</v>
-      </c>
-      <c r="H38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>7135</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39">
-        <v>0.1</v>
-      </c>
-      <c r="G39">
-        <v>10</v>
-      </c>
-      <c r="H39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>7136</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40">
-        <v>0.1</v>
-      </c>
-      <c r="G40">
-        <v>10</v>
-      </c>
-      <c r="H40">
-        <v>10</v>
+    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>7137</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>7138</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>7139</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>